<commit_message>
pushing before further changing model in case need to revert to previous model
</commit_message>
<xml_diff>
--- a/Model 12_16/10_25_2017 cost parameters.xlsx
+++ b/Model 12_16/10_25_2017 cost parameters.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amber\Documents\Carbapenem\Carbapenem-Resistance\Model 12_16\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amber\Documents\Yale\CIDMA\AMR\Carbapenem-Resistance\Model 12_16\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7200" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7200" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Sheet5" sheetId="5" r:id="rId4"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -894,7 +894,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="14">
     <numFmt numFmtId="164" formatCode="#\ ???/???"/>
     <numFmt numFmtId="165" formatCode="#\ ??/11"/>
@@ -1538,26 +1538,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K51"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="K54" sqref="C47:K54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="2"/>
-    <col min="4" max="4" width="6.140625" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.140625" style="2"/>
-    <col min="9" max="9" width="6.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.453125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" style="2"/>
+    <col min="4" max="4" width="6.1796875" customWidth="1"/>
+    <col min="5" max="5" width="8.81640625" customWidth="1"/>
+    <col min="6" max="6" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.1796875" style="2"/>
+    <col min="9" max="9" width="6.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1566,7 +1566,7 @@
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -1595,7 +1595,7 @@
       </c>
       <c r="K2" s="10"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>41</v>
       </c>
@@ -1624,7 +1624,7 @@
       </c>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>41</v>
       </c>
@@ -1653,7 +1653,7 @@
       </c>
       <c r="K4" s="10"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>41</v>
       </c>
@@ -1682,7 +1682,7 @@
       </c>
       <c r="K5" s="10"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>41</v>
       </c>
@@ -1711,7 +1711,7 @@
       </c>
       <c r="K6" s="10"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>41</v>
       </c>
@@ -1740,7 +1740,7 @@
       </c>
       <c r="K7" s="10"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>41</v>
       </c>
@@ -1769,7 +1769,7 @@
       </c>
       <c r="K8" s="10"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>41</v>
       </c>
@@ -1801,7 +1801,7 @@
       </c>
       <c r="K9" s="10"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>41</v>
       </c>
@@ -1833,7 +1833,7 @@
       </c>
       <c r="K10" s="10"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="2" t="s">
         <v>135</v>
@@ -1859,7 +1859,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
         <v>3</v>
       </c>
@@ -1893,7 +1893,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="6"/>
       <c r="B13" s="2" t="s">
         <v>136</v>
@@ -1923,7 +1923,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>41</v>
       </c>
@@ -1957,7 +1957,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>41</v>
       </c>
@@ -1991,7 +1991,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>41</v>
       </c>
@@ -2025,7 +2025,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>41</v>
       </c>
@@ -2059,7 +2059,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>41</v>
       </c>
@@ -2092,7 +2092,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>41</v>
       </c>
@@ -2126,7 +2126,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>41</v>
       </c>
@@ -2160,7 +2160,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>41</v>
       </c>
@@ -2181,7 +2181,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
         <v>4</v>
       </c>
@@ -2215,7 +2215,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>41</v>
       </c>
@@ -2236,7 +2236,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>41</v>
       </c>
@@ -2244,7 +2244,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>41</v>
       </c>
@@ -2252,7 +2252,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>41</v>
       </c>
@@ -2260,7 +2260,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>41</v>
       </c>
@@ -2268,12 +2268,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="F30" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="7" t="s">
         <v>62</v>
       </c>
@@ -2281,7 +2281,7 @@
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="6" t="s">
         <v>1</v>
       </c>
@@ -2309,7 +2309,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>41</v>
       </c>
@@ -2337,7 +2337,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>41</v>
       </c>
@@ -2365,7 +2365,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>41</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>41</v>
       </c>
@@ -2421,7 +2421,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>41</v>
       </c>
@@ -2452,7 +2452,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>41</v>
       </c>
@@ -2486,7 +2486,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="6" t="s">
         <v>3</v>
       </c>
@@ -2520,7 +2520,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>41</v>
       </c>
@@ -2554,7 +2554,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>41</v>
       </c>
@@ -2588,7 +2588,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
@@ -2609,7 +2609,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>41</v>
       </c>
@@ -2617,7 +2617,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>41</v>
       </c>
@@ -2625,7 +2625,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" s="6" t="s">
         <v>4</v>
       </c>
@@ -2646,7 +2646,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>41</v>
       </c>
@@ -2654,7 +2654,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>41</v>
       </c>
@@ -2662,7 +2662,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>41</v>
       </c>
@@ -2670,7 +2670,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>41</v>
       </c>
@@ -2678,7 +2678,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>41</v>
       </c>
@@ -2686,7 +2686,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F51" s="2"/>
     </row>
   </sheetData>
@@ -2696,22 +2696,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J67"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.140625" style="2"/>
-    <col min="6" max="6" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.140625" style="2"/>
+    <col min="1" max="1" width="13.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.1796875" style="2"/>
+    <col min="6" max="6" width="13.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2721,7 +2721,7 @@
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
@@ -2735,7 +2735,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>41</v>
       </c>
@@ -2766,7 +2766,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>41</v>
       </c>
@@ -2797,7 +2797,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>41</v>
       </c>
@@ -2825,7 +2825,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>41</v>
       </c>
@@ -2853,7 +2853,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>41</v>
       </c>
@@ -2881,7 +2881,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>41</v>
       </c>
@@ -2909,7 +2909,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
         <v>101</v>
       </c>
@@ -2931,7 +2931,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>1</v>
       </c>
@@ -2952,7 +2952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>41</v>
       </c>
@@ -2960,7 +2960,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>41</v>
       </c>
@@ -2968,7 +2968,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>41</v>
       </c>
@@ -2976,7 +2976,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>41</v>
       </c>
@@ -2984,7 +2984,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>41</v>
       </c>
@@ -2992,7 +2992,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
         <v>3</v>
       </c>
@@ -3013,7 +3013,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>41</v>
       </c>
@@ -3021,7 +3021,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>41</v>
       </c>
@@ -3029,7 +3029,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>41</v>
       </c>
@@ -3037,7 +3037,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>41</v>
       </c>
@@ -3045,7 +3045,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>41</v>
       </c>
@@ -3053,7 +3053,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
         <v>2</v>
       </c>
@@ -3061,7 +3061,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>41</v>
       </c>
@@ -3069,7 +3069,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>41</v>
       </c>
@@ -3077,7 +3077,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>41</v>
       </c>
@@ -3085,7 +3085,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>41</v>
       </c>
@@ -3093,7 +3093,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>41</v>
       </c>
@@ -3101,7 +3101,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="6" t="s">
         <v>3</v>
       </c>
@@ -3109,7 +3109,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>41</v>
       </c>
@@ -3117,7 +3117,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>41</v>
       </c>
@@ -3125,7 +3125,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>41</v>
       </c>
@@ -3133,7 +3133,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>41</v>
       </c>
@@ -3141,7 +3141,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>41</v>
       </c>
@@ -3149,7 +3149,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="7" t="s">
         <v>62</v>
       </c>
@@ -3159,7 +3159,7 @@
       <c r="G37" s="8"/>
       <c r="H37" s="8"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="6" t="s">
         <v>4</v>
       </c>
@@ -3187,7 +3187,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>41</v>
       </c>
@@ -3215,7 +3215,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>41</v>
       </c>
@@ -3243,7 +3243,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>41</v>
       </c>
@@ -3271,7 +3271,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
@@ -3279,7 +3279,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>41</v>
       </c>
@@ -3287,7 +3287,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" s="6" t="s">
         <v>1</v>
       </c>
@@ -3308,7 +3308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>41</v>
       </c>
@@ -3316,7 +3316,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>41</v>
       </c>
@@ -3324,7 +3324,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>41</v>
       </c>
@@ -3332,7 +3332,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>41</v>
       </c>
@@ -3340,7 +3340,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>41</v>
       </c>
@@ -3348,7 +3348,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" s="6" t="s">
         <v>3</v>
       </c>
@@ -3369,7 +3369,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>41</v>
       </c>
@@ -3377,7 +3377,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>41</v>
       </c>
@@ -3385,7 +3385,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>41</v>
       </c>
@@ -3393,7 +3393,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>41</v>
       </c>
@@ -3401,7 +3401,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>41</v>
       </c>
@@ -3409,7 +3409,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" s="6" t="s">
         <v>2</v>
       </c>
@@ -3417,7 +3417,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>41</v>
       </c>
@@ -3425,7 +3425,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>41</v>
       </c>
@@ -3433,7 +3433,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>41</v>
       </c>
@@ -3441,7 +3441,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>41</v>
       </c>
@@ -3449,7 +3449,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>41</v>
       </c>
@@ -3457,7 +3457,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" s="6" t="s">
         <v>3</v>
       </c>
@@ -3465,7 +3465,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>41</v>
       </c>
@@ -3473,7 +3473,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>41</v>
       </c>
@@ -3481,7 +3481,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>41</v>
       </c>
@@ -3489,7 +3489,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>41</v>
       </c>
@@ -3497,7 +3497,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>41</v>
       </c>
@@ -3511,32 +3511,32 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" style="55" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" style="55" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="55"/>
-    <col min="4" max="4" width="20.5703125" style="55" customWidth="1"/>
-    <col min="5" max="5" width="66.85546875" style="55" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" style="55" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="55" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="55"/>
-    <col min="9" max="9" width="17.7109375" style="55" customWidth="1"/>
-    <col min="10" max="10" width="76.7109375" style="55" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="55"/>
+    <col min="1" max="1" width="13.453125" style="55" customWidth="1"/>
+    <col min="2" max="2" width="9.26953125" style="55" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" style="55"/>
+    <col min="4" max="4" width="20.54296875" style="55" customWidth="1"/>
+    <col min="5" max="5" width="66.81640625" style="55" customWidth="1"/>
+    <col min="6" max="6" width="14.1796875" style="55" customWidth="1"/>
+    <col min="7" max="7" width="12.453125" style="55" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.1796875" style="55"/>
+    <col min="9" max="9" width="17.7265625" style="55" customWidth="1"/>
+    <col min="10" max="10" width="76.7265625" style="55" customWidth="1"/>
+    <col min="11" max="16384" width="9.1796875" style="55"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
@@ -3550,7 +3550,7 @@
       <c r="I1" s="54"/>
       <c r="J1" s="54"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="56" t="s">
         <v>1</v>
       </c>
@@ -3579,7 +3579,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="61" t="s">
         <v>41</v>
       </c>
@@ -3610,7 +3610,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="61" t="s">
         <v>41</v>
       </c>
@@ -3639,7 +3639,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" s="64" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="62" t="s">
         <v>41</v>
       </c>
@@ -3668,7 +3668,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="67" t="s">
         <v>41</v>
       </c>
@@ -3697,7 +3697,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="61" t="s">
         <v>41</v>
       </c>
@@ -3726,7 +3726,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="61" t="s">
         <v>41</v>
       </c>
@@ -3755,7 +3755,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="61" t="s">
         <v>41</v>
       </c>
@@ -3786,7 +3786,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" s="64" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="62"/>
       <c r="B10" s="63" t="s">
         <v>135</v>
@@ -3813,7 +3813,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="69" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" s="69" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="67" t="s">
         <v>41</v>
       </c>
@@ -3842,7 +3842,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" s="64" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="70" t="s">
         <v>3</v>
       </c>
@@ -3876,7 +3876,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="56"/>
       <c r="B13" s="58" t="s">
         <v>136</v>
@@ -3906,7 +3906,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="61" t="s">
         <v>41</v>
       </c>
@@ -3940,7 +3940,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="64" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" s="64" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="62" t="s">
         <v>41</v>
       </c>
@@ -3974,7 +3974,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="67" t="s">
         <v>41</v>
       </c>
@@ -4008,7 +4008,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="61" t="s">
         <v>41</v>
       </c>
@@ -4042,7 +4042,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="61" t="s">
         <v>41</v>
       </c>
@@ -4076,7 +4076,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A19" s="61" t="s">
         <v>41</v>
       </c>
@@ -4110,7 +4110,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="61" t="s">
         <v>41</v>
       </c>
@@ -4131,7 +4131,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="77" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" s="77" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="75" t="s">
         <v>41</v>
       </c>
@@ -4164,7 +4164,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="64" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" s="64" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="70" t="s">
         <v>4</v>
       </c>
@@ -4198,7 +4198,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="61" t="s">
         <v>41</v>
       </c>
@@ -4221,7 +4221,7 @@
       <c r="G23" s="58"/>
       <c r="H23" s="58"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="61" t="s">
         <v>41</v>
       </c>
@@ -4233,7 +4233,7 @@
       <c r="G24" s="58"/>
       <c r="H24" s="58"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="61" t="s">
         <v>41</v>
       </c>
@@ -4245,7 +4245,7 @@
       <c r="G25" s="58"/>
       <c r="H25" s="58"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="61" t="s">
         <v>41</v>
       </c>
@@ -4260,7 +4260,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="61" t="s">
         <v>41</v>
       </c>
@@ -4272,10 +4272,10 @@
       <c r="G27" s="58"/>
       <c r="H27" s="58"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="G28" s="79"/>
     </row>
-    <row r="35" spans="1:11" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" s="54" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="52" t="s">
         <v>62</v>
       </c>
@@ -4283,7 +4283,7 @@
       <c r="G35" s="53"/>
       <c r="H35" s="53"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" s="56" t="s">
         <v>1</v>
       </c>
@@ -4312,7 +4312,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37" s="61" t="s">
         <v>41</v>
       </c>
@@ -4341,7 +4341,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38" s="61" t="s">
         <v>41</v>
       </c>
@@ -4370,7 +4370,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39" s="61" t="s">
         <v>41</v>
       </c>
@@ -4399,7 +4399,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" s="61" t="s">
         <v>41</v>
       </c>
@@ -4428,7 +4428,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41" s="61" t="s">
         <v>41</v>
       </c>
@@ -4459,7 +4459,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42" s="61" t="s">
         <v>41</v>
       </c>
@@ -4494,7 +4494,7 @@
       </c>
       <c r="K42" s="60"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43" s="56" t="s">
         <v>3</v>
       </c>
@@ -4528,7 +4528,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44" s="61" t="s">
         <v>41</v>
       </c>
@@ -4562,7 +4562,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A45" s="61" t="s">
         <v>41</v>
       </c>
@@ -4596,7 +4596,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A46" s="61" t="s">
         <v>41</v>
       </c>
@@ -4619,7 +4619,7 @@
       <c r="G46" s="58"/>
       <c r="H46" s="58"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47" s="61" t="s">
         <v>41</v>
       </c>
@@ -4631,7 +4631,7 @@
       <c r="G47" s="58"/>
       <c r="H47" s="58"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48" s="61" t="s">
         <v>41</v>
       </c>
@@ -4643,7 +4643,7 @@
       <c r="G48" s="58"/>
       <c r="H48" s="58"/>
     </row>
-    <row r="49" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A49" s="56" t="s">
         <v>4</v>
       </c>
@@ -4673,25 +4673,25 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.140625" style="2"/>
-    <col min="8" max="8" width="6.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="6.1796875" customWidth="1"/>
+    <col min="4" max="4" width="12.26953125" customWidth="1"/>
+    <col min="5" max="5" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.1796875" style="2"/>
+    <col min="8" max="8" width="6.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -4699,7 +4699,7 @@
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
     </row>
-    <row r="2" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="80" t="s">
         <v>1</v>
       </c>
@@ -4710,7 +4710,7 @@
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>244</v>
       </c>
@@ -4728,12 +4728,12 @@
       </c>
       <c r="G3" s="9"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="6"/>
       <c r="E4" s="6"/>
       <c r="G4" s="9"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>41</v>
       </c>
@@ -4741,7 +4741,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>41</v>
       </c>
@@ -4749,7 +4749,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>41</v>
       </c>
@@ -4759,7 +4759,7 @@
       </c>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>41</v>
       </c>
@@ -4767,7 +4767,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>41</v>
       </c>
@@ -4775,7 +4775,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>41</v>
       </c>
@@ -4784,7 +4784,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>41</v>
       </c>
@@ -4793,7 +4793,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>41</v>
       </c>
@@ -4802,7 +4802,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
         <v>4</v>
       </c>
@@ -4819,7 +4819,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>41</v>
       </c>
@@ -4836,7 +4836,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>41</v>
       </c>
@@ -4844,7 +4844,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>41</v>
       </c>
@@ -4852,7 +4852,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>41</v>
       </c>
@@ -4860,7 +4860,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>41</v>
       </c>
@@ -4868,14 +4868,14 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>62</v>
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="80" t="s">
         <v>1</v>
       </c>
@@ -4886,7 +4886,7 @@
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
         <v>244</v>
       </c>
@@ -4904,12 +4904,12 @@
       </c>
       <c r="G21" s="9"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="6"/>
       <c r="E22" s="6"/>
       <c r="G22" s="9"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>41</v>
       </c>
@@ -4917,7 +4917,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>41</v>
       </c>
@@ -4925,7 +4925,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>41</v>
       </c>
@@ -4935,7 +4935,7 @@
       </c>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>41</v>
       </c>
@@ -4943,7 +4943,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>41</v>
       </c>
@@ -4951,7 +4951,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>41</v>
       </c>
@@ -4960,7 +4960,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>41</v>
       </c>
@@ -4969,7 +4969,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>41</v>
       </c>
@@ -4978,7 +4978,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="6" t="s">
         <v>4</v>
       </c>
@@ -4995,7 +4995,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>41</v>
       </c>
@@ -5012,7 +5012,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>41</v>
       </c>
@@ -5020,7 +5020,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>41</v>
       </c>
@@ -5028,7 +5028,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>41</v>
       </c>
@@ -5036,7 +5036,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>41</v>
       </c>
@@ -5044,160 +5044,160 @@
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="80"/>
       <c r="B37" s="9"/>
       <c r="F37" s="9"/>
       <c r="G37" s="9"/>
     </row>
-    <row r="38" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="81"/>
       <c r="B38" s="9"/>
       <c r="E38" s="81"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9"/>
     </row>
-    <row r="39" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="81"/>
       <c r="B39" s="9"/>
       <c r="E39" s="81"/>
       <c r="F39" s="9"/>
       <c r="G39" s="9"/>
     </row>
-    <row r="40" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="80"/>
       <c r="B40" s="9"/>
       <c r="E40" s="80"/>
       <c r="F40" s="9"/>
       <c r="G40" s="9"/>
     </row>
-    <row r="41" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="80"/>
       <c r="B41" s="9"/>
       <c r="E41" s="80"/>
       <c r="F41" s="9"/>
       <c r="G41" s="9"/>
     </row>
-    <row r="42" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="80"/>
       <c r="B42" s="82"/>
       <c r="E42" s="80"/>
       <c r="F42" s="82"/>
       <c r="G42" s="9"/>
     </row>
-    <row r="43" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43" s="80"/>
       <c r="B43" s="9"/>
       <c r="E43" s="80"/>
       <c r="F43" s="9"/>
       <c r="G43" s="9"/>
     </row>
-    <row r="44" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44" s="80"/>
       <c r="B44" s="9"/>
       <c r="E44" s="80"/>
       <c r="F44" s="9"/>
       <c r="G44" s="9"/>
     </row>
-    <row r="45" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A45" s="80"/>
       <c r="B45" s="83"/>
       <c r="E45" s="80"/>
       <c r="F45" s="9"/>
       <c r="G45" s="9"/>
     </row>
-    <row r="46" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="80"/>
       <c r="B46" s="83"/>
       <c r="E46" s="80"/>
       <c r="F46" s="9"/>
       <c r="G46" s="9"/>
     </row>
-    <row r="47" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="80"/>
       <c r="B47" s="83"/>
       <c r="E47" s="80"/>
       <c r="F47" s="9"/>
       <c r="G47" s="9"/>
     </row>
-    <row r="48" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A48" s="81"/>
       <c r="B48" s="82"/>
       <c r="E48" s="81"/>
       <c r="F48" s="9"/>
       <c r="G48" s="9"/>
     </row>
-    <row r="49" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="80"/>
       <c r="B49" s="9"/>
       <c r="E49" s="80"/>
       <c r="F49" s="9"/>
       <c r="G49" s="9"/>
     </row>
-    <row r="50" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="80"/>
       <c r="B50" s="9"/>
       <c r="E50" s="80"/>
       <c r="F50" s="9"/>
       <c r="G50" s="9"/>
     </row>
-    <row r="51" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="80"/>
       <c r="B51" s="9"/>
       <c r="E51" s="80"/>
       <c r="F51" s="9"/>
       <c r="G51" s="9"/>
     </row>
-    <row r="52" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A52" s="80"/>
       <c r="B52" s="9"/>
       <c r="E52" s="80"/>
       <c r="F52" s="9"/>
       <c r="G52" s="9"/>
     </row>
-    <row r="53" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A53" s="80"/>
       <c r="B53" s="9"/>
       <c r="E53" s="80"/>
       <c r="F53" s="9"/>
       <c r="G53" s="9"/>
     </row>
-    <row r="54" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B54" s="9"/>
       <c r="F54" s="9"/>
       <c r="G54" s="9"/>
     </row>
-    <row r="55" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B55" s="9"/>
       <c r="F55" s="9"/>
       <c r="G55" s="9"/>
     </row>
-    <row r="56" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B56" s="9"/>
       <c r="F56" s="9"/>
       <c r="G56" s="9"/>
     </row>
-    <row r="57" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B57" s="9"/>
       <c r="F57" s="9"/>
       <c r="G57" s="9"/>
     </row>
-    <row r="58" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B58" s="9"/>
       <c r="F58" s="9"/>
       <c r="G58" s="9"/>
     </row>
-    <row r="59" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B59" s="9"/>
       <c r="F59" s="9"/>
       <c r="G59" s="9"/>
     </row>
-    <row r="60" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B60" s="9"/>
       <c r="F60" s="9"/>
       <c r="G60" s="9"/>
     </row>
-    <row r="61" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B61" s="9"/>
       <c r="F61" s="9"/>
       <c r="G61" s="9"/>
@@ -5208,50 +5208,50 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AO48"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K58" sqref="K58"/>
+    <sheetView tabSelected="1" topLeftCell="Q4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="W29" sqref="W29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" style="11" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="19"/>
-    <col min="3" max="3" width="9.140625" style="12"/>
-    <col min="4" max="4" width="9.140625" style="19"/>
-    <col min="5" max="5" width="9.140625" style="12"/>
-    <col min="6" max="6" width="14.85546875" style="19" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" style="12" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="11"/>
-    <col min="10" max="10" width="11.140625" style="19" customWidth="1"/>
-    <col min="11" max="11" width="23.28515625" style="22" customWidth="1"/>
+    <col min="1" max="1" width="22.81640625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="9.1796875" style="19"/>
+    <col min="3" max="3" width="9.1796875" style="12"/>
+    <col min="4" max="4" width="9.1796875" style="19"/>
+    <col min="5" max="5" width="9.1796875" style="12"/>
+    <col min="6" max="6" width="14.81640625" style="19" customWidth="1"/>
+    <col min="7" max="7" width="17.453125" style="12" customWidth="1"/>
+    <col min="8" max="8" width="11.54296875" style="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.1796875" style="11"/>
+    <col min="10" max="10" width="11.1796875" style="19" customWidth="1"/>
+    <col min="11" max="11" width="23.26953125" style="22" customWidth="1"/>
     <col min="12" max="12" width="12" style="19" customWidth="1"/>
     <col min="13" max="13" width="23" style="12" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" style="19" customWidth="1"/>
+    <col min="14" max="14" width="10.54296875" style="19" customWidth="1"/>
     <col min="15" max="15" width="28" style="12" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" style="19"/>
-    <col min="17" max="17" width="28.5703125" style="11" customWidth="1"/>
-    <col min="18" max="18" width="9.140625" style="19"/>
-    <col min="19" max="21" width="9.140625" style="12"/>
-    <col min="22" max="22" width="18.85546875" style="19" customWidth="1"/>
+    <col min="16" max="16" width="9.1796875" style="19"/>
+    <col min="17" max="17" width="28.54296875" style="11" customWidth="1"/>
+    <col min="18" max="18" width="9.1796875" style="19"/>
+    <col min="19" max="21" width="9.1796875" style="12"/>
+    <col min="22" max="22" width="18.81640625" style="19" customWidth="1"/>
     <col min="23" max="23" width="17" style="12" customWidth="1"/>
-    <col min="24" max="24" width="12.85546875" style="19" customWidth="1"/>
-    <col min="25" max="25" width="18.42578125" style="11" customWidth="1"/>
-    <col min="26" max="26" width="9.140625" style="19"/>
-    <col min="27" max="27" width="9.140625" style="12"/>
-    <col min="28" max="28" width="9.140625" style="19"/>
-    <col min="29" max="29" width="9.140625" style="12"/>
-    <col min="30" max="30" width="11.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9.140625" style="12"/>
-    <col min="32" max="32" width="9.140625" style="19"/>
-    <col min="33" max="33" width="9.140625" style="11"/>
-    <col min="34" max="16384" width="9.140625" style="12"/>
+    <col min="24" max="24" width="12.81640625" style="19" customWidth="1"/>
+    <col min="25" max="25" width="18.453125" style="11" customWidth="1"/>
+    <col min="26" max="26" width="9.1796875" style="19"/>
+    <col min="27" max="27" width="9.1796875" style="12"/>
+    <col min="28" max="28" width="9.1796875" style="19"/>
+    <col min="29" max="29" width="9.1796875" style="12"/>
+    <col min="30" max="30" width="11.54296875" style="19" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.1796875" style="12"/>
+    <col min="32" max="32" width="9.1796875" style="19"/>
+    <col min="33" max="33" width="9.1796875" style="11"/>
+    <col min="34" max="16384" width="9.1796875" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.35">
       <c r="B1" s="84" t="s">
         <v>142</v>
       </c>
@@ -5303,7 +5303,7 @@
       <c r="AN1" s="84"/>
       <c r="AO1" s="84"/>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.35">
       <c r="B2" s="84" t="s">
         <v>147</v>
       </c>
@@ -5385,7 +5385,7 @@
       </c>
       <c r="AO2" s="84"/>
     </row>
-    <row r="3" spans="1:41" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:41" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13"/>
       <c r="B3" s="14" t="s">
         <v>150</v>
@@ -5508,7 +5508,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A4" s="18" t="s">
         <v>152</v>
       </c>
@@ -5544,7 +5544,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="5" spans="1:41" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:41" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="26"/>
       <c r="B5" s="27"/>
       <c r="D5" s="27"/>
@@ -5571,7 +5571,7 @@
       <c r="AF5" s="27"/>
       <c r="AG5" s="13"/>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A6" s="31" t="s">
         <v>158</v>
       </c>
@@ -5608,7 +5608,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A7" s="31"/>
       <c r="F7" s="20"/>
       <c r="H7" s="20" t="s">
@@ -5626,7 +5626,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A8" s="31"/>
       <c r="F8" s="20"/>
       <c r="H8" s="20" t="s">
@@ -5644,7 +5644,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="9" spans="1:41" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:41" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="32"/>
       <c r="B9" s="27"/>
       <c r="D9" s="27"/>
@@ -5675,7 +5675,7 @@
       <c r="AF9" s="27"/>
       <c r="AG9" s="13"/>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A10" s="34" t="s">
         <v>180</v>
       </c>
@@ -5711,7 +5711,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A11" s="34"/>
       <c r="F11" s="20"/>
       <c r="H11" s="20"/>
@@ -5730,7 +5730,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:41" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:41" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="38"/>
       <c r="B12" s="27"/>
       <c r="D12" s="27"/>
@@ -5757,7 +5757,7 @@
       <c r="AF12" s="27"/>
       <c r="AG12" s="13"/>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A13" s="34" t="s">
         <v>186</v>
       </c>
@@ -5783,7 +5783,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:41" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:41" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="38"/>
       <c r="B14" s="27"/>
       <c r="D14" s="27"/>
@@ -5810,7 +5810,7 @@
       <c r="AF14" s="27"/>
       <c r="AG14" s="13"/>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A15" s="31" t="s">
         <v>187</v>
       </c>
@@ -5842,7 +5842,7 @@
       </c>
       <c r="X15" s="42"/>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A16" s="31"/>
       <c r="F16" s="20"/>
       <c r="H16" s="43">
@@ -5861,7 +5861,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A17" s="31"/>
       <c r="F17" s="20"/>
       <c r="H17" s="41"/>
@@ -5875,7 +5875,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A18" s="31"/>
       <c r="F18" s="20"/>
       <c r="H18" s="41"/>
@@ -5892,7 +5892,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="19" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="32"/>
       <c r="B19" s="27"/>
       <c r="D19" s="27"/>
@@ -5914,7 +5914,7 @@
       <c r="AF19" s="27"/>
       <c r="AG19" s="13"/>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A20" s="34" t="s">
         <v>180</v>
       </c>
@@ -5950,7 +5950,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A21" s="34"/>
       <c r="F21" s="20"/>
       <c r="J21" s="20"/>
@@ -5963,7 +5963,7 @@
       </c>
       <c r="V21" s="20"/>
     </row>
-    <row r="22" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="38"/>
       <c r="B22" s="27"/>
       <c r="D22" s="27"/>
@@ -5990,7 +5990,7 @@
       <c r="AF22" s="27"/>
       <c r="AG22" s="13"/>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A23" s="34" t="s">
         <v>186</v>
       </c>
@@ -6014,7 +6014,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="13"/>
       <c r="B24" s="27"/>
       <c r="D24" s="27"/>
@@ -6036,7 +6036,7 @@
       <c r="AF24" s="27"/>
       <c r="AG24" s="13"/>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A25" s="18" t="s">
         <v>204</v>
       </c>
@@ -6045,7 +6045,7 @@
       <c r="N25" s="20"/>
       <c r="V25" s="20"/>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A26" s="31" t="s">
         <v>158</v>
       </c>
@@ -6082,7 +6082,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A27" s="31"/>
       <c r="F27" s="20" t="s">
         <v>209</v>
@@ -6098,7 +6098,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A28" s="31"/>
       <c r="F28" s="20" t="s">
         <v>212</v>
@@ -6115,7 +6115,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="29" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="32"/>
       <c r="B29" s="27"/>
       <c r="D29" s="27"/>
@@ -6142,7 +6142,7 @@
       <c r="AF29" s="27"/>
       <c r="AG29" s="13"/>
     </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A30" s="34" t="s">
         <v>180</v>
       </c>
@@ -6162,7 +6162,7 @@
       </c>
       <c r="V30" s="20"/>
     </row>
-    <row r="31" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="38"/>
       <c r="B31" s="27"/>
       <c r="D31" s="27"/>
@@ -6189,7 +6189,7 @@
       <c r="AF31" s="27"/>
       <c r="AG31" s="13"/>
     </row>
-    <row r="32" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="38" t="s">
         <v>186</v>
       </c>
@@ -6213,7 +6213,7 @@
       <c r="AF32" s="27"/>
       <c r="AG32" s="13"/>
     </row>
-    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A33" s="31" t="s">
         <v>187</v>
       </c>
@@ -6244,7 +6244,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A34" s="31"/>
       <c r="F34" s="20" t="s">
         <v>226</v>
@@ -6261,7 +6261,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A35" s="31"/>
       <c r="F35" s="20" t="s">
         <v>228</v>
@@ -6278,7 +6278,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="36" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="32"/>
       <c r="B36" s="27"/>
       <c r="D36" s="27"/>
@@ -6305,7 +6305,7 @@
       <c r="AF36" s="27"/>
       <c r="AG36" s="13"/>
     </row>
-    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A37" s="34" t="s">
         <v>180</v>
       </c>
@@ -6325,7 +6325,7 @@
       </c>
       <c r="V37" s="20"/>
     </row>
-    <row r="38" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="38"/>
       <c r="B38" s="27"/>
       <c r="D38" s="27"/>
@@ -6352,7 +6352,7 @@
       <c r="AF38" s="27"/>
       <c r="AG38" s="13"/>
     </row>
-    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A39" s="34" t="s">
         <v>186</v>
       </c>
@@ -6361,12 +6361,12 @@
       <c r="O39" s="50"/>
       <c r="V39" s="20"/>
     </row>
-    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:33" x14ac:dyDescent="0.35">
       <c r="F40" s="20"/>
       <c r="L40" s="20"/>
       <c r="V40" s="20"/>
     </row>
-    <row r="41" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="13"/>
       <c r="B41" s="27"/>
       <c r="D41" s="27"/>
@@ -6388,7 +6388,7 @@
       <c r="AF41" s="27"/>
       <c r="AG41" s="13"/>
     </row>
-    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A42" s="18" t="s">
         <v>236</v>
       </c>
@@ -6418,30 +6418,39 @@
         <v>49</v>
       </c>
     </row>
-    <row r="43" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:33" x14ac:dyDescent="0.35">
       <c r="F43" s="20"/>
       <c r="L43" s="20"/>
     </row>
-    <row r="44" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:33" x14ac:dyDescent="0.35">
       <c r="F44" s="20"/>
       <c r="V44" s="20"/>
     </row>
-    <row r="45" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:33" x14ac:dyDescent="0.35">
       <c r="F45" s="20"/>
       <c r="L45" s="20"/>
       <c r="V45" s="20"/>
     </row>
-    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:33" x14ac:dyDescent="0.35">
       <c r="L46" s="20"/>
     </row>
-    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:33" x14ac:dyDescent="0.35">
       <c r="K47" s="50"/>
     </row>
-    <row r="48" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:33" x14ac:dyDescent="0.35">
       <c r="O48" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="AJ2:AK2"/>
+    <mergeCell ref="AL2:AM2"/>
+    <mergeCell ref="AN2:AO2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AF2:AG2"/>
+    <mergeCell ref="AH2:AI2"/>
     <mergeCell ref="AH1:AO1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -6458,15 +6467,6 @@
     <mergeCell ref="P2:Q2"/>
     <mergeCell ref="R2:S2"/>
     <mergeCell ref="T2:U2"/>
-    <mergeCell ref="AJ2:AK2"/>
-    <mergeCell ref="AL2:AM2"/>
-    <mergeCell ref="AN2:AO2"/>
-    <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="AF2:AG2"/>
-    <mergeCell ref="AH2:AI2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>